<commit_message>
fix timing bug at end of the day
</commit_message>
<xml_diff>
--- a/cloudfun/day-1/CloudCore-FY21-Day-1-americas.xlsx
+++ b/cloudfun/day-1/CloudCore-FY21-Day-1-americas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanPatrick\DB\Dropbox (Personal)\GitHub\cloud-core-2020-fix2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanPatrick\DB\Dropbox (Personal)\GitHub\cloud-core-2020-fix2\cloudfun\day-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82B6A904-B017-43FB-B8A0-2BE0F98020DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4736AAD-127E-4824-9860-CB14E3759B6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{0B725299-4060-418E-A1A8-086098773DCE}"/>
   </bookViews>
@@ -821,7 +821,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1719,7 @@
         <v>0.92708333333333315</v>
       </c>
       <c r="H28" s="13">
-        <v>5.2083333333333336E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>32</v>
@@ -1742,30 +1742,30 @@
       </c>
       <c r="B29" s="6">
         <f t="shared" si="0"/>
-        <v>0.56249999999999978</v>
+        <v>0.57291666666666652</v>
       </c>
       <c r="C29" s="38">
         <f t="shared" si="1"/>
-        <v>0.68749999999999978</v>
+        <v>0.69791666666666641</v>
       </c>
       <c r="D29" s="38">
         <f t="shared" si="4"/>
-        <v>0.64583333333333315</v>
+        <v>0.65624999999999978</v>
       </c>
       <c r="E29" s="38">
         <f t="shared" si="2"/>
-        <v>0.68749999999999978</v>
+        <v>0.69791666666666641</v>
       </c>
       <c r="F29" s="23">
         <f t="shared" si="5"/>
-        <v>0.89583333333333315</v>
+        <v>0.90624999999999978</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="3"/>
-        <v>0.97916666666666652</v>
+        <v>0.98958333333333315</v>
       </c>
       <c r="H29" s="13">
-        <v>7.2916666666666671E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>33</v>
@@ -1788,27 +1788,27 @@
       </c>
       <c r="B30" s="6">
         <f t="shared" si="0"/>
-        <v>0.63541666666666652</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="C30" s="38">
         <f t="shared" si="1"/>
-        <v>0.76041666666666641</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="D30" s="38">
         <f t="shared" si="4"/>
-        <v>0.71874999999999978</v>
+        <v>0.66666666666666641</v>
       </c>
       <c r="E30" s="38">
         <f t="shared" si="2"/>
-        <v>0.76041666666666641</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="F30" s="23">
         <f t="shared" si="5"/>
-        <v>0.96874999999999978</v>
+        <v>0.91666666666666641</v>
       </c>
       <c r="G30" s="7">
         <f t="shared" si="3"/>
-        <v>5.2083333333333037E-2</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="H30" s="13">
         <v>1.0416666666666666E-2</v>

</xml_diff>

<commit_message>
Upgrade from Ciprian to Lino
</commit_message>
<xml_diff>
--- a/cloudfun/day-1/CloudCore-FY21-Day-1-americas.xlsx
+++ b/cloudfun/day-1/CloudCore-FY21-Day-1-americas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanPatrick\DB\Dropbox (Personal)\GitHub\cloud-core-2020-fix2\cloudfun\day-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4736AAD-127E-4824-9860-CB14E3759B6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC8F7B-DCE0-400C-A457-DD1BDBFCBB43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{0B725299-4060-418E-A1A8-086098773DCE}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>Ben</t>
   </si>
   <si>
-    <t>Ciprian (week 1) Lino (Week 2)</t>
-  </si>
-  <si>
     <t>Instructors in Breakout Rooms</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>UTC</t>
+  </si>
+  <si>
+    <t>Lino</t>
   </si>
 </sst>
 </file>
@@ -821,7 +821,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -870,22 +870,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>1</v>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="9" t="s">
@@ -1676,13 +1676,13 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
@@ -1722,13 +1722,13 @@
         <v>6.25E-2</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
@@ -1768,13 +1768,13 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="37"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
@@ -1814,7 +1814,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>

</xml_diff>